<commit_message>
Added progress bar - not interactive yet
</commit_message>
<xml_diff>
--- a/TestFile.xlsx
+++ b/TestFile.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kim\Documents\College\Summer 2018\B6 Animation\time_machine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kimmy\Documents\College\Summer 2018\B6 Animation\time_machine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0A1254EC-2913-4D27-83E5-3617EE0565D2}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{9DE24BF2-70F2-446C-BD3D-D8B80C59F1EE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -370,11 +369,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D02C57F7-B454-47FE-8ED0-0B9B433F1633}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added preliminary `click to navigate` feature to progress bar
</commit_message>
<xml_diff>
--- a/TestFile.xlsx
+++ b/TestFile.xlsx
@@ -370,121 +370,151 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
         <v>0.1</v>
       </c>
-      <c r="B1">
+      <c r="C1">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="D1">
         <v>0.5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
         <v>0.2</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>0.9</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
         <v>0.3</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>0.8</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
         <v>0.4</v>
-      </c>
-      <c r="B4">
-        <v>0.7</v>
       </c>
       <c r="C4">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
         <v>0.5</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>0.6</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>0.3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
         <v>0.6</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>0.5</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>0.6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
         <v>0.7</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>0.4</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>0.9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
         <v>0.8</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>0.3</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
         <v>0.9</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>0.2</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>0.4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
         <v>1</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>0.1</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>0.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added option to import data point labels from spreadsheet
</commit_message>
<xml_diff>
--- a/TestFile.xlsx
+++ b/TestFile.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kimmy\Documents\College\Summer 2018\B6 Animation\time_machine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kim\Documents\College\Summer 2018\B6 Animation\time_machine\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F447A4E5-A0E4-4F2D-97F4-B744A1B82E85}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,8 +24,25 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>One</t>
+  </si>
+  <si>
+    <t>Two</t>
+  </si>
+  <si>
+    <t>Three</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -369,152 +387,166 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1">
-        <v>0.1</v>
-      </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <v>0.5</v>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="C2">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
+        <v>0.2</v>
+      </c>
+      <c r="C3">
+        <v>0.9</v>
+      </c>
+      <c r="D3">
         <v>0.3</v>
-      </c>
-      <c r="C3">
-        <v>0.8</v>
-      </c>
-      <c r="D3">
-        <v>0.2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="C4">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="D4">
-        <v>0.7</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C5">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="D5">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
+        <v>0.5</v>
+      </c>
+      <c r="C6">
         <v>0.6</v>
       </c>
-      <c r="C6">
-        <v>0.5</v>
-      </c>
       <c r="D6">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="C7">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="D7">
-        <v>0.9</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="C8">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="D8">
-        <v>0.1</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="C9">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="D9">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>0.9</v>
+      </c>
+      <c r="C10">
+        <v>0.2</v>
+      </c>
+      <c r="D10">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>1</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <v>0.1</v>
       </c>
-      <c r="D10">
+      <c r="D11">
         <v>0.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added ability to add arrows by dragging between to data points - no animation functionality yet
</commit_message>
<xml_diff>
--- a/TestFile.xlsx
+++ b/TestFile.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kim\Documents\College\Summer 2018\B6 Animation\time_machine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kimmy\Documents\College\Summer 2018\B6 Animation\time_machine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F447A4E5-A0E4-4F2D-97F4-B744A1B82E85}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B1643132-E793-46BE-AE01-F1B8AB6B12EE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -391,7 +391,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Arrows now move with data point movement and change color based on data point data - still need to add specific flux data
</commit_message>
<xml_diff>
--- a/TestFile.xlsx
+++ b/TestFile.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kimmy\Documents\College\Summer 2018\B6 Animation\time_machine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B1643132-E793-46BE-AE01-F1B8AB6B12EE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B442E14A-293C-48B1-BB1B-C3DF5ECE38F0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="5">
   <si>
     <t>t</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>Three</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Two </t>
   </si>
 </sst>
 </file>
@@ -388,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="A14" sqref="A14:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,87 +470,129 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>0.5</v>
-      </c>
-      <c r="C6">
-        <v>0.6</v>
-      </c>
-      <c r="D6">
-        <v>0.3</v>
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
+        <v>0.5</v>
+      </c>
+      <c r="C7">
         <v>0.6</v>
       </c>
-      <c r="C7">
-        <v>0.5</v>
-      </c>
       <c r="D7">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="C8">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="D8">
-        <v>0.9</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>0.8</v>
-      </c>
-      <c r="C9">
-        <v>0.3</v>
-      </c>
-      <c r="D9">
-        <v>0.1</v>
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10">
+        <v>0.7</v>
+      </c>
+      <c r="C10">
+        <v>0.4</v>
+      </c>
+      <c r="D10">
         <v>0.9</v>
-      </c>
-      <c r="C10">
-        <v>0.2</v>
-      </c>
-      <c r="D10">
-        <v>0.4</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>0.8</v>
+      </c>
+      <c r="C11">
+        <v>0.3</v>
+      </c>
+      <c r="D11">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>0.9</v>
+      </c>
+      <c r="C12">
+        <v>0.2</v>
+      </c>
+      <c r="D12">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B13">
         <v>1</v>
       </c>
-      <c r="C11">
+      <c r="C13">
         <v>0.1</v>
       </c>
-      <c r="D11">
+      <c r="D13">
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjust progress bar and improved compartment generation
</commit_message>
<xml_diff>
--- a/TestFile.xlsx
+++ b/TestFile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kimmy\Documents\College\Summer 2018\B6 Animation\time_machine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B442E14A-293C-48B1-BB1B-C3DF5ECE38F0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B63E14F-9DD8-45CE-B3C0-DEFB25F06DB9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -394,7 +394,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:D14"/>
+      <selection activeCell="D1" sqref="A1:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>